<commit_message>
counting change, fix some bugs
</commit_message>
<xml_diff>
--- a/metalDB.xlsx
+++ b/metalDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\HollowSecCalculator\v0.7\calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91530F41-A623-44B6-BC93-079309A04117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FEEEB0-0BC4-44DD-A422-30E2C14C9F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,9 +384,6 @@
     <t>IPE750x196</t>
   </si>
   <si>
-    <t>CH76x38x7</t>
-  </si>
-  <si>
     <t>CH102x51x10</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>CH432x102x65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH76x38x7 </t>
   </si>
 </sst>
 </file>
@@ -736,48 +736,6 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="5" tint="0.39997558519241921"/>
@@ -814,6 +772,48 @@
           <bgColor theme="5"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1454,7 +1454,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8451F2FA-F1C6-4EAD-A2E1-E614B8D01A4C}" name="Table9" displayName="Table9" ref="A1:G18" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8451F2FA-F1C6-4EAD-A2E1-E614B8D01A4C}" name="Table9" displayName="Table9" ref="A1:G18" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3">
   <autoFilter ref="A1:G18" xr:uid="{8451F2FA-F1C6-4EAD-A2E1-E614B8D01A4C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{63F59C3B-C90C-4970-93E9-038EDA8BA758}" name="N"/>
@@ -1470,7 +1470,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{38506F01-E960-459C-927A-1C1572B9A216}" name="Table6" displayName="Table6" ref="A1:D190" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{38506F01-E960-459C-927A-1C1572B9A216}" name="Table6" displayName="Table6" ref="A1:D190" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:D190" xr:uid="{38506F01-E960-459C-927A-1C1572B9A216}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{841719B2-8EB9-440E-B847-9BA84F5357D5}" name="W"/>
@@ -1748,7 +1748,7 @@
   <dimension ref="A1:D218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4818,7 +4818,7 @@
   <dimension ref="A1:D307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9133,8 +9133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C7F4A8-E037-4A4F-8AAD-32E383D53875}">
   <dimension ref="A1:C216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187:C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13990,8 +13990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04F7681-8F2C-4235-BB99-A2A6DC9F639B}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16190,7 +16190,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16619,7 +16619,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16652,7 +16652,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="B2">
         <v>6.7</v>
@@ -16675,7 +16675,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3">
         <v>10.4</v>
@@ -16698,7 +16698,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4">
         <v>14.9</v>
@@ -16721,7 +16721,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <v>17.899999999999999</v>
@@ -16744,7 +16744,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <v>23.9</v>
@@ -16767,7 +16767,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>20.8</v>
@@ -16790,7 +16790,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8">
         <v>26.8</v>
@@ -16813,7 +16813,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9">
         <v>23.9</v>
@@ -16836,7 +16836,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10">
         <v>29.8</v>
@@ -16859,7 +16859,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11">
         <v>26.1</v>
@@ -16882,7 +16882,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12">
         <v>32.700000000000003</v>
@@ -16905,7 +16905,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13">
         <v>28.2</v>
@@ -16928,7 +16928,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14">
         <v>35.700000000000003</v>
@@ -16951,7 +16951,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B15">
         <v>41.8</v>
@@ -16974,7 +16974,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16">
         <v>46.2</v>
@@ -16997,7 +16997,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17">
         <v>55</v>
@@ -17020,7 +17020,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18">
         <v>65.5</v>

</xml_diff>